<commit_message>
--Data Validation Module - Documentation Update--
README.MD was updated to updated the links to the Centralized Cruise Database (CCD: git@gitlab.pifsc.gov:centralized-data-tools/centralized-cruise-database.git) and CCD DVM documentation
updated docs\DVM - Business Rules.xlsx to add a column "Test Case Exists" to indicate if there is a corresponding DVM test case for the given processing error code ("Scope" column value is DVM Processing Errors") due to an update in the CCD DVM testing documentation
</commit_message>
<xml_diff>
--- a/docs/DVM - Business Rules.xlsx
+++ b/docs/DVM - Business Rules.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="122">
   <si>
     <t>Rule Description</t>
   </si>
@@ -376,6 +376,15 @@
   </si>
   <si>
     <t>The DVM was not successfully processed</t>
+  </si>
+  <si>
+    <t>Test Case Exists? (if applicable)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -419,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -432,6 +441,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,11 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,11 +734,11 @@
     <col min="1" max="3" width="24.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="86" style="2" customWidth="1"/>
     <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
-    <col min="6" max="11" width="24.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="12" width="24.42578125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -753,29 +763,32 @@
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -798,8 +811,11 @@
       <c r="G2" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
@@ -823,8 +839,11 @@
       <c r="G3" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -847,8 +866,11 @@
       <c r="G4" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A13" si="1">A4+1</f>
         <v>4</v>
@@ -872,8 +894,11 @@
       <c r="G5" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -897,8 +922,11 @@
       <c r="G6" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -922,8 +950,11 @@
       <c r="G7" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -947,8 +978,11 @@
       <c r="G8" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -972,8 +1006,11 @@
       <c r="G9" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -997,8 +1034,11 @@
       <c r="G10" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1022,8 +1062,11 @@
       <c r="G11" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1047,8 +1090,11 @@
       <c r="G12" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1072,8 +1118,11 @@
       <c r="G13" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1097,8 +1146,11 @@
       <c r="G14" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="I14" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f>A14+1</f>
         <v>2</v>
@@ -1123,8 +1175,11 @@
       <c r="G15" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="I15" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" ref="A16:A27" si="5">A15+1</f>
         <v>3</v>
@@ -1149,8 +1204,11 @@
       <c r="G16" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I16" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -1175,8 +1233,11 @@
       <c r="G17" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I17" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -1201,8 +1262,11 @@
       <c r="G18" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I18" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -1227,8 +1291,11 @@
       <c r="G19" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I19" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -1253,8 +1320,11 @@
       <c r="G20" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I20" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -1279,8 +1349,11 @@
       <c r="G21" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -1305,8 +1378,11 @@
       <c r="G22" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I22" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="5"/>
         <v>10</v>
@@ -1330,8 +1406,11 @@
       <c r="G23" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="5"/>
         <v>11</v>
@@ -1355,8 +1434,11 @@
       <c r="G24" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="5"/>
         <v>12</v>
@@ -1381,8 +1463,11 @@
       <c r="G25" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I25" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="5"/>
         <v>13</v>
@@ -1407,8 +1492,11 @@
       <c r="G26" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="I26" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="5"/>
         <v>14</v>
@@ -1433,8 +1521,11 @@
       <c r="G27" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I27" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -1457,8 +1548,11 @@
       <c r="G28" s="2">
         <v>-20200</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>A28+1</f>
         <v>2</v>
@@ -1482,8 +1576,11 @@
       <c r="G29" s="2">
         <v>-20201</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I29" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" ref="A30:A44" si="11">A29+1</f>
         <v>3</v>
@@ -1508,8 +1605,11 @@
       <c r="G30" s="2">
         <v>-20202</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I30" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="11"/>
         <v>4</v>
@@ -1534,8 +1634,11 @@
       <c r="G31" s="2">
         <v>-20203</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I31" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="11"/>
         <v>5</v>
@@ -1559,8 +1662,11 @@
       <c r="G32" s="2">
         <v>-20204</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I32" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="11"/>
         <v>6</v>
@@ -1584,8 +1690,11 @@
       <c r="G33" s="2">
         <v>-20205</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I33" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="11"/>
         <v>7</v>
@@ -1609,8 +1718,11 @@
       <c r="G34" s="2">
         <v>-20206</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I34" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="11"/>
         <v>8</v>
@@ -1634,8 +1746,11 @@
       <c r="G35" s="2">
         <v>-20207</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I35" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="11"/>
         <v>9</v>
@@ -1659,8 +1774,11 @@
       <c r="G36" s="2">
         <v>-20208</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I36" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="11"/>
         <v>10</v>
@@ -1684,8 +1802,11 @@
       <c r="G37" s="2">
         <v>-20209</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I37" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="11"/>
         <v>11</v>
@@ -1710,8 +1831,11 @@
       <c r="G38" s="2">
         <v>-20210</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I38" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="11"/>
         <v>12</v>
@@ -1736,8 +1860,11 @@
       <c r="G39" s="2">
         <v>-20211</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I39" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="11"/>
         <v>13</v>
@@ -1761,8 +1888,11 @@
       <c r="G40" s="2">
         <v>-20212</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I40" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="11"/>
         <v>14</v>
@@ -1786,8 +1916,11 @@
       <c r="G41" s="2">
         <v>-20213</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I41" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="11"/>
         <v>15</v>
@@ -1811,8 +1944,11 @@
       <c r="G42" s="2">
         <v>-20214</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I42" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="11"/>
         <v>16</v>
@@ -1836,8 +1972,11 @@
       <c r="G43" s="2">
         <v>-20215</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I43" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="11"/>
         <v>17</v>
@@ -1861,8 +2000,11 @@
       <c r="G44" s="2">
         <v>-20216</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I44" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" ref="A45:A60" si="12">A44+1</f>
         <v>18</v>
@@ -1886,8 +2028,11 @@
       <c r="G45" s="2">
         <v>-20217</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I45" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f t="shared" si="12"/>
         <v>19</v>
@@ -1911,8 +2056,11 @@
       <c r="G46" s="2">
         <v>-20218</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I46" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f t="shared" si="12"/>
         <v>20</v>
@@ -1936,8 +2084,11 @@
       <c r="G47" s="2">
         <v>-20219</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f t="shared" si="12"/>
         <v>21</v>
@@ -1962,8 +2113,11 @@
       <c r="G48" s="2">
         <v>-20220</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f t="shared" si="12"/>
         <v>22</v>
@@ -1988,8 +2142,11 @@
       <c r="G49" s="2">
         <v>-20221</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I49" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" si="12"/>
         <v>23</v>
@@ -2013,8 +2170,11 @@
       <c r="G50" s="2">
         <v>-20222</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I50" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="12"/>
         <v>24</v>
@@ -2038,8 +2198,11 @@
       <c r="G51" s="2">
         <v>-20223</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I51" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="12"/>
         <v>25</v>
@@ -2064,8 +2227,11 @@
       <c r="G52" s="2">
         <v>-20224</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I52" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="12"/>
         <v>26</v>
@@ -2090,8 +2256,11 @@
       <c r="G53" s="2">
         <v>-20225</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I53" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="12"/>
         <v>27</v>
@@ -2115,8 +2284,11 @@
       <c r="G54" s="2">
         <v>-20226</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I54" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f t="shared" si="12"/>
         <v>28</v>
@@ -2140,8 +2312,11 @@
       <c r="G55" s="2">
         <v>-20227</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I55" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="12"/>
         <v>29</v>
@@ -2165,8 +2340,11 @@
       <c r="G56" s="2">
         <v>-20228</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I56" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f t="shared" si="12"/>
         <v>30</v>
@@ -2190,8 +2368,11 @@
       <c r="G57" s="2">
         <v>-20229</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I57" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f t="shared" si="12"/>
         <v>31</v>
@@ -2215,8 +2396,11 @@
       <c r="G58" s="2">
         <v>-20230</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I58" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f t="shared" si="12"/>
         <v>32</v>
@@ -2240,8 +2424,11 @@
       <c r="G59" s="2">
         <v>-20231</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="I59" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <f t="shared" si="12"/>
         <v>33</v>
@@ -2266,8 +2453,11 @@
       <c r="G60" s="2">
         <v>-20232</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I60" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <f t="shared" ref="A61:A65" si="13">A60+1</f>
         <v>34</v>
@@ -2291,8 +2481,11 @@
       <c r="G61" s="2">
         <v>-20233</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="I61" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="13"/>
         <v>35</v>
@@ -2317,8 +2510,11 @@
       <c r="G62" s="2">
         <v>-20234</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I62" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <f t="shared" si="13"/>
         <v>36</v>
@@ -2343,8 +2539,11 @@
       <c r="G63" s="2">
         <v>-20235</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="I63" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="13"/>
         <v>37</v>
@@ -2369,8 +2568,11 @@
       <c r="G64" s="2">
         <v>-20236</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="13"/>
         <v>38</v>
@@ -2393,6 +2595,9 @@
       </c>
       <c r="G65" s="2">
         <v>-20237</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>